<commit_message>
Add pipeline for scraping full forecast tables to Postgres
</commit_message>
<xml_diff>
--- a/scrape_mountain_weather_data/src/current-weather.xlsx
+++ b/scrape_mountain_weather_data/src/current-weather.xlsx
@@ -470,7 +470,7 @@
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>forecast_local_time</t>
+          <t>local_time_of_forecast</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>45375.50555555556</v>
+        <v>45375.51041666666</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>45375.45833333334</v>

</xml_diff>